<commit_message>
TOPIC_TABLE COLUMNS TOPIC_TEXT ADD
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
   <si>
     <t>Home Page</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>UNIQUE</t>
+  </si>
+  <si>
+    <t>TOPIC_TEXT</t>
+  </si>
+  <si>
+    <t>VARCHAR(3000)</t>
   </si>
 </sst>
 </file>
@@ -232,6 +238,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -241,11 +249,9 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,17 +636,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
       <c r="D1" s="5"/>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
       <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -742,119 +748,125 @@
       <c r="J6" s="6"/>
     </row>
     <row r="8" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="10"/>
+      <c r="D9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
     </row>
     <row r="11" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="10"/>
+      <c r="D11" s="7"/>
     </row>
     <row r="12" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B13" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="10"/>
-    </row>
-    <row r="13" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B14" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10" t="s">
+      <c r="C14" s="7"/>
+      <c r="D14" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-    </row>
     <row r="16" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="8"/>
     </row>
     <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="12"/>
+      <c r="D17" s="8"/>
     </row>
     <row r="18" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="12"/>
+      <c r="D18" s="8"/>
     </row>
     <row r="19" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>